<commit_message>
Update many statistics for February 2025
</commit_message>
<xml_diff>
--- a/statistics_files/2025/2025_99_y_graph.xlsx
+++ b/statistics_files/2025/2025_99_y_graph.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\George\Documents\github\next_statistics\statistics_files\2025\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD14305F-4F35-4145-9B68-9E88BA0F422E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C87C585-A1A9-424A-B454-4FDED5AFBAB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1004,6 +1004,9 @@
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>81653</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>77057</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1280,7 +1283,7 @@
                   <c:showPercent val="0"/>
                   <c:showBubbleSize val="0"/>
                   <c:showLeaderLines val="0"/>
-                  <c:extLst>
+                  <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                     <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                       <c15:showLeaderLines val="1"/>
                       <c15:leaderLines>
@@ -1308,7 +1311,7 @@
                     </c:pt>
                   </c:numLit>
                 </c:val>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000001-9EB2-4B94-ABEF-053018645AEE}"/>
                   </c:ext>
@@ -2379,7 +2382,7 @@
   <dimension ref="A1:G30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2451,6 +2454,9 @@
       </c>
       <c r="F3">
         <v>84080</v>
+      </c>
+      <c r="G3">
+        <v>77057</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Update all files for March 2025
</commit_message>
<xml_diff>
--- a/statistics_files/2025/2025_99_y_graph.xlsx
+++ b/statistics_files/2025/2025_99_y_graph.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\George\Documents\github\next_statistics\statistics_files\2025\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C87C585-A1A9-424A-B454-4FDED5AFBAB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7ACD8DB1-2A9B-4972-9E3F-B1C2CD4403EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1007,6 +1007,9 @@
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>77057</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>87177</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2382,7 +2385,7 @@
   <dimension ref="A1:G30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2477,6 +2480,9 @@
       </c>
       <c r="F4">
         <v>89067</v>
+      </c>
+      <c r="G4">
+        <v>87177</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
First part of July statistics
</commit_message>
<xml_diff>
--- a/statistics_files/2025/2025_99_y_graph.xlsx
+++ b/statistics_files/2025/2025_99_y_graph.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\George\Documents\github\next_statistics\statistics_files\2025\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E1063B6-0D95-4E0A-9B7E-BA53056CAF8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{771E9809-B2F3-46C5-B626-36DA8AED655C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1019,6 +1019,9 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>103033</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>102146</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2393,8 +2396,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2581,6 +2584,9 @@
       </c>
       <c r="F8">
         <v>107365</v>
+      </c>
+      <c r="G8">
+        <v>102146</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Update images and monthly overview
</commit_message>
<xml_diff>
--- a/statistics_files/2025/2025_99_y_graph.xlsx
+++ b/statistics_files/2025/2025_99_y_graph.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24334"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20417"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\George\Documents\github\next_statistics\statistics_files\2025\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E047121E-F472-4CDB-8F03-997014E3AF91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C1E5374-EE51-425A-A5C5-FB1FDE1E1190}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -19,15 +19,6 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:xlwcv="http://schemas.microsoft.com/office/spreadsheetml/2024/workbookCompatibilityVersion" uri="{D14903EA-33C4-47F7-8F05-3474C54BE107}">
       <xlwcv:version setVersion="1"/>
@@ -1037,6 +1028,9 @@
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>89988</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>88575</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2412,7 +2406,7 @@
   <dimension ref="A1:G30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2645,6 +2639,9 @@
       </c>
       <c r="F10">
         <v>83710</v>
+      </c>
+      <c r="G10">
+        <v>88575</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Update svg and graph files for October, 2025
</commit_message>
<xml_diff>
--- a/statistics_files/2025/2025_99_y_graph.xlsx
+++ b/statistics_files/2025/2025_99_y_graph.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20417"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24334"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\George\Documents\github\next_statistics\statistics_files\2025\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C1E5374-EE51-425A-A5C5-FB1FDE1E1190}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D3D1746-BC37-4D5B-B947-B5835941A78E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1031,6 +1031,9 @@
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>88575</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>90165</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2406,7 +2409,7 @@
   <dimension ref="A1:G30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2662,6 +2665,9 @@
       </c>
       <c r="F11">
         <v>88412</v>
+      </c>
+      <c r="G11">
+        <v>90165</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Update overview, executive board, graph and svg files
</commit_message>
<xml_diff>
--- a/statistics_files/2025/2025_99_y_graph.xlsx
+++ b/statistics_files/2025/2025_99_y_graph.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\George\Documents\github\next_statistics\statistics_files\2025\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D3D1746-BC37-4D5B-B947-B5835941A78E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75BD4322-08A0-4A13-A1AD-8956F0044E8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1034,6 +1034,9 @@
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>90165</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>75089</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2409,7 +2412,7 @@
   <dimension ref="A1:G30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2688,6 +2691,9 @@
       </c>
       <c r="F12">
         <v>77799</v>
+      </c>
+      <c r="G12">
+        <v>75089</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Update graph and executive board statistics
</commit_message>
<xml_diff>
--- a/statistics_files/2025/2025_99_y_graph.xlsx
+++ b/statistics_files/2025/2025_99_y_graph.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\George\Documents\github\next_statistics\statistics_files\2025\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75BD4322-08A0-4A13-A1AD-8956F0044E8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBD5EF86-2BA9-4B9F-A41E-750E528B74EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1036,6 +1036,9 @@
                   <c:v>90165</c:v>
                 </c:pt>
                 <c:pt idx="10">
+                  <c:v>75089</c:v>
+                </c:pt>
+                <c:pt idx="11">
                   <c:v>75089</c:v>
                 </c:pt>
               </c:numCache>
@@ -2412,7 +2415,7 @@
   <dimension ref="A1:G30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2714,6 +2717,9 @@
       </c>
       <c r="F13">
         <v>89666</v>
+      </c>
+      <c r="G13">
+        <v>75089</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>